<commit_message>
Aggiunta feature per non avere problemi sul .pdf finale
</commit_message>
<xml_diff>
--- a/CercaPdf/cerca.xlsx
+++ b/CercaPdf/cerca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Haider Maqsood\Desktop\Software\CercaPdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C161C8D1-2612-43BE-8895-5EA5CEC19ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3B3B5F-FDBA-4751-BBF3-38DE7A47252E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2355" windowWidth="20730" windowHeight="11160" xr2:uid="{E3CF18D8-7B63-4772-892E-5AA85ED10D84}"/>
   </bookViews>
@@ -30,10 +30,10 @@
     <t>cercare</t>
   </si>
   <si>
-    <t>find1</t>
+    <t>notfind2</t>
   </si>
   <si>
-    <t>notfind2</t>
+    <t>find1.pdf</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,12 +403,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>